<commit_message>
update all chnaged and new files to github
</commit_message>
<xml_diff>
--- a/ClearView_Mester_Demo_Data_2025_11_01.xlsx
+++ b/ClearView_Mester_Demo_Data_2025_11_01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4100" tabRatio="774" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4100" tabRatio="774" firstSheet="9" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Paths" sheetId="26" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5409" uniqueCount="1429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5411" uniqueCount="1431">
   <si>
     <t>Expense_Holder</t>
   </si>
@@ -4360,6 +4360,12 @@
   </si>
   <si>
     <t>Salary-Om</t>
+  </si>
+  <si>
+    <t>Invested_Amount</t>
+  </si>
+  <si>
+    <t>Expected_Amount</t>
   </si>
 </sst>
 </file>
@@ -8882,10 +8888,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8904,7 +8910,7 @@
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>464</v>
       </c>
@@ -8941,8 +8947,14 @@
       <c r="L1" s="1" t="s">
         <v>1251</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -8980,7 +8992,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>470</v>
       </c>
@@ -9015,7 +9027,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>472</v>
       </c>
@@ -9053,7 +9065,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>475</v>
       </c>
@@ -9088,7 +9100,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>478</v>
       </c>
@@ -9123,7 +9135,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>479</v>
       </c>
@@ -9161,7 +9173,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>482</v>
       </c>
@@ -9196,7 +9208,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>484</v>
       </c>
@@ -9231,7 +9243,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>486</v>
       </c>
@@ -9266,7 +9278,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>488</v>
       </c>
@@ -9301,7 +9313,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>489</v>
       </c>
@@ -9336,7 +9348,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>491</v>
       </c>
@@ -9371,7 +9383,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>493</v>
       </c>
@@ -9406,7 +9418,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>495</v>
       </c>
@@ -9441,7 +9453,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>497</v>
       </c>
@@ -21270,7 +21282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+    <sheetView topLeftCell="A92" workbookViewId="0">
       <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>

</xml_diff>